<commit_message>
some fix for numeric value
</commit_message>
<xml_diff>
--- a/t/format_test_sheet.xlsx
+++ b/t/format_test_sheet.xlsx
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>文字列</t>
+  </si>
+  <si>
+    <t>biginteger</t>
   </si>
 </sst>
 </file>
@@ -214,6 +217,14 @@
         <v>13</v>
       </c>
     </row>
+    <row r="11">
+      <c t="s" s="1" r="A11">
+        <v>14</v>
+      </c>
+      <c s="1" r="B11">
+        <v>1.25702689E8</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>